<commit_message>
8 wafer added in list (to be tested)
</commit_message>
<xml_diff>
--- a/waferstatus_20150612.xlsx
+++ b/waferstatus_20150612.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="15135" windowHeight="9300" tabRatio="281"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$54:$L$78</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="293">
   <si>
     <t>Wafer</t>
   </si>
@@ -868,16 +868,46 @@
   </si>
   <si>
     <t>Waferstatus 12.06.2015 (PSI46dig V2.1respin)</t>
+  </si>
+  <si>
+    <t>8 Stück</t>
+  </si>
+  <si>
+    <t>4KSGB00000</t>
+  </si>
+  <si>
+    <t>VR6CD9X</t>
+  </si>
+  <si>
+    <t>VS6CD8X</t>
+  </si>
+  <si>
+    <t>VS6CH6X</t>
+  </si>
+  <si>
+    <t>VM6CDDX</t>
+  </si>
+  <si>
+    <t>VT6CD7X</t>
+  </si>
+  <si>
+    <t>VP6CDBX</t>
+  </si>
+  <si>
+    <t>VS6CEQX</t>
+  </si>
+  <si>
+    <t>VN6CDCX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1090,7 +1120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1196,26 +1226,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1274,7 +1289,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1296,9 +1310,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1311,9 +1326,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1351,7 +1366,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1385,6 +1400,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1419,9 +1435,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1594,20 +1611,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:P169"/>
+  <dimension ref="B1:P151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="N111" sqref="N111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
     <col min="2" max="2" width="3.140625" style="25" customWidth="1"/>
@@ -1624,21 +1641,21 @@
     <col min="13" max="256" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="23.25">
-      <c r="D1" s="87" t="s">
+    <row r="1" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D1" s="81" t="s">
         <v>282</v>
       </c>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-    </row>
-    <row r="2" spans="2:16" ht="6.75" customHeight="1"/>
-    <row r="3" spans="2:16" s="12" customFormat="1">
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+    </row>
+    <row r="2" spans="2:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="27"/>
       <c r="C3" s="13" t="s">
         <v>101</v>
@@ -1670,21 +1687,21 @@
       <c r="L3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="65" t="s">
+      <c r="M3" s="60" t="s">
         <v>271</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="62" t="s">
         <v>268</v>
       </c>
-      <c r="O3" s="67" t="s">
+      <c r="O3" s="62" t="s">
         <v>269</v>
       </c>
-      <c r="P3" s="66" t="s">
+      <c r="P3" s="61" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="12.75" customHeight="1">
-      <c r="B4" s="84" t="s">
+    <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="78" t="s">
         <v>172</v>
       </c>
       <c r="C4" s="31">
@@ -1707,13 +1724,13 @@
       <c r="L4" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="M4" s="62"/>
+      <c r="M4" s="57"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="63"/>
-    </row>
-    <row r="5" spans="2:16">
-      <c r="B5" s="85"/>
+      <c r="P4" s="58"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B5" s="79"/>
       <c r="C5" s="32">
         <v>2</v>
       </c>
@@ -1734,13 +1751,13 @@
       <c r="L5" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="M5" s="62"/>
+      <c r="M5" s="57"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="63"/>
-    </row>
-    <row r="6" spans="2:16">
-      <c r="B6" s="85"/>
+      <c r="P5" s="58"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B6" s="79"/>
       <c r="C6" s="32">
         <v>3</v>
       </c>
@@ -1761,13 +1778,13 @@
       <c r="L6" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="M6" s="62"/>
+      <c r="M6" s="57"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="63"/>
-    </row>
-    <row r="7" spans="2:16">
-      <c r="B7" s="85"/>
+      <c r="P6" s="58"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="79"/>
       <c r="C7" s="32">
         <v>4</v>
       </c>
@@ -1788,13 +1805,13 @@
       <c r="L7" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="M7" s="62"/>
+      <c r="M7" s="57"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="63"/>
-    </row>
-    <row r="8" spans="2:16">
-      <c r="B8" s="85"/>
+      <c r="P7" s="58"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B8" s="79"/>
       <c r="C8" s="32">
         <v>5</v>
       </c>
@@ -1815,13 +1832,13 @@
       <c r="L8" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="M8" s="62"/>
+      <c r="M8" s="57"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="63"/>
-    </row>
-    <row r="9" spans="2:16">
-      <c r="B9" s="85"/>
+      <c r="P8" s="58"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B9" s="79"/>
       <c r="C9" s="32">
         <v>6</v>
       </c>
@@ -1845,13 +1862,13 @@
       <c r="J9" s="8"/>
       <c r="K9" s="15"/>
       <c r="L9" s="34"/>
-      <c r="M9" s="62"/>
+      <c r="M9" s="57"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="63"/>
-    </row>
-    <row r="10" spans="2:16">
-      <c r="B10" s="85"/>
+      <c r="P9" s="58"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="79"/>
       <c r="C10" s="32">
         <v>7</v>
       </c>
@@ -1875,13 +1892,13 @@
       <c r="J10" s="8"/>
       <c r="K10" s="15"/>
       <c r="L10" s="34"/>
-      <c r="M10" s="62"/>
+      <c r="M10" s="57"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="63"/>
-    </row>
-    <row r="11" spans="2:16">
-      <c r="B11" s="85"/>
+      <c r="P10" s="58"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B11" s="79"/>
       <c r="C11" s="32">
         <v>8</v>
       </c>
@@ -1905,13 +1922,13 @@
       <c r="J11" s="8"/>
       <c r="K11" s="15"/>
       <c r="L11" s="34"/>
-      <c r="M11" s="62"/>
+      <c r="M11" s="57"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="63"/>
-    </row>
-    <row r="12" spans="2:16">
-      <c r="B12" s="85"/>
+      <c r="P11" s="58"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B12" s="79"/>
       <c r="C12" s="32">
         <v>9</v>
       </c>
@@ -1935,13 +1952,13 @@
       <c r="J12" s="8"/>
       <c r="K12" s="15"/>
       <c r="L12" s="34"/>
-      <c r="M12" s="62"/>
+      <c r="M12" s="57"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="63"/>
-    </row>
-    <row r="13" spans="2:16">
-      <c r="B13" s="85"/>
+      <c r="P12" s="58"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B13" s="79"/>
       <c r="C13" s="32">
         <v>10</v>
       </c>
@@ -1967,13 +1984,13 @@
       <c r="L13" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="M13" s="62"/>
+      <c r="M13" s="57"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="63"/>
-    </row>
-    <row r="14" spans="2:16">
-      <c r="B14" s="85"/>
+      <c r="P13" s="58"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B14" s="79"/>
       <c r="C14" s="32">
         <v>11</v>
       </c>
@@ -1999,13 +2016,13 @@
       <c r="L14" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="M14" s="62"/>
+      <c r="M14" s="57"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="63"/>
-    </row>
-    <row r="15" spans="2:16">
-      <c r="B15" s="85"/>
+      <c r="P14" s="58"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B15" s="79"/>
       <c r="C15" s="32">
         <v>12</v>
       </c>
@@ -2031,13 +2048,13 @@
       <c r="L15" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="M15" s="62"/>
+      <c r="M15" s="57"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="63"/>
-    </row>
-    <row r="16" spans="2:16">
-      <c r="B16" s="85"/>
+      <c r="P15" s="58"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B16" s="79"/>
       <c r="C16" s="32">
         <v>13</v>
       </c>
@@ -2063,13 +2080,13 @@
       <c r="L16" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="M16" s="62"/>
+      <c r="M16" s="57"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="63"/>
-    </row>
-    <row r="17" spans="2:16">
-      <c r="B17" s="85"/>
+      <c r="P16" s="58"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B17" s="79"/>
       <c r="C17" s="32">
         <v>14</v>
       </c>
@@ -2095,13 +2112,13 @@
       <c r="L17" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="M17" s="62"/>
+      <c r="M17" s="57"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="63"/>
-    </row>
-    <row r="18" spans="2:16">
-      <c r="B18" s="85"/>
+      <c r="P17" s="58"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B18" s="79"/>
       <c r="C18" s="32">
         <v>15</v>
       </c>
@@ -2125,13 +2142,13 @@
       <c r="J18" s="8"/>
       <c r="K18" s="15"/>
       <c r="L18" s="34"/>
-      <c r="M18" s="62"/>
+      <c r="M18" s="57"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="63"/>
-    </row>
-    <row r="19" spans="2:16">
-      <c r="B19" s="85"/>
+      <c r="P18" s="58"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B19" s="79"/>
       <c r="C19" s="32">
         <v>16</v>
       </c>
@@ -2155,13 +2172,13 @@
       <c r="J19" s="8"/>
       <c r="K19" s="15"/>
       <c r="L19" s="34"/>
-      <c r="M19" s="62"/>
+      <c r="M19" s="57"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="63"/>
-    </row>
-    <row r="20" spans="2:16">
-      <c r="B20" s="85"/>
+      <c r="P19" s="58"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B20" s="79"/>
       <c r="C20" s="32">
         <v>17</v>
       </c>
@@ -2185,13 +2202,13 @@
       <c r="J20" s="8"/>
       <c r="K20" s="15"/>
       <c r="L20" s="34"/>
-      <c r="M20" s="62"/>
+      <c r="M20" s="57"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="63"/>
-    </row>
-    <row r="21" spans="2:16">
-      <c r="B21" s="85"/>
+      <c r="P20" s="58"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B21" s="79"/>
       <c r="C21" s="32">
         <v>18</v>
       </c>
@@ -2215,13 +2232,13 @@
       <c r="J21" s="8"/>
       <c r="K21" s="15"/>
       <c r="L21" s="34"/>
-      <c r="M21" s="62"/>
+      <c r="M21" s="57"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="63"/>
-    </row>
-    <row r="22" spans="2:16">
-      <c r="B22" s="85"/>
+      <c r="P21" s="58"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B22" s="79"/>
       <c r="C22" s="32">
         <v>19</v>
       </c>
@@ -2245,13 +2262,13 @@
       <c r="J22" s="8"/>
       <c r="K22" s="15"/>
       <c r="L22" s="34"/>
-      <c r="M22" s="62"/>
+      <c r="M22" s="57"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="63"/>
-    </row>
-    <row r="23" spans="2:16">
-      <c r="B23" s="85"/>
+      <c r="P22" s="58"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B23" s="79"/>
       <c r="C23" s="32">
         <v>20</v>
       </c>
@@ -2275,13 +2292,13 @@
       <c r="J23" s="8"/>
       <c r="K23" s="15"/>
       <c r="L23" s="34"/>
-      <c r="M23" s="62"/>
+      <c r="M23" s="57"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="63"/>
-    </row>
-    <row r="24" spans="2:16">
-      <c r="B24" s="85"/>
+      <c r="P23" s="58"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B24" s="79"/>
       <c r="C24" s="32">
         <v>21</v>
       </c>
@@ -2305,13 +2322,13 @@
       <c r="J24" s="8"/>
       <c r="K24" s="15"/>
       <c r="L24" s="34"/>
-      <c r="M24" s="62"/>
+      <c r="M24" s="57"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="63"/>
-    </row>
-    <row r="25" spans="2:16">
-      <c r="B25" s="85"/>
+      <c r="P24" s="58"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B25" s="79"/>
       <c r="C25" s="32">
         <v>22</v>
       </c>
@@ -2335,13 +2352,13 @@
       <c r="J25" s="8"/>
       <c r="K25" s="15"/>
       <c r="L25" s="34"/>
-      <c r="M25" s="62"/>
+      <c r="M25" s="57"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="63"/>
-    </row>
-    <row r="26" spans="2:16">
-      <c r="B26" s="85"/>
+      <c r="P25" s="58"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B26" s="79"/>
       <c r="C26" s="32">
         <v>23</v>
       </c>
@@ -2364,13 +2381,13 @@
       <c r="J26" s="8"/>
       <c r="K26" s="15"/>
       <c r="L26" s="34"/>
-      <c r="M26" s="62"/>
+      <c r="M26" s="57"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="63"/>
-    </row>
-    <row r="27" spans="2:16">
-      <c r="B27" s="85"/>
+      <c r="P26" s="58"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B27" s="79"/>
       <c r="C27" s="32">
         <v>24</v>
       </c>
@@ -2396,13 +2413,13 @@
       </c>
       <c r="K27" s="15"/>
       <c r="L27" s="34"/>
-      <c r="M27" s="62"/>
+      <c r="M27" s="57"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="63"/>
-    </row>
-    <row r="28" spans="2:16" s="12" customFormat="1">
-      <c r="B28" s="86"/>
+      <c r="P27" s="58"/>
+    </row>
+    <row r="28" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="80"/>
       <c r="C28" s="33">
         <v>25</v>
       </c>
@@ -2428,25 +2445,25 @@
       </c>
       <c r="K28" s="16"/>
       <c r="L28" s="35"/>
-      <c r="M28" s="69">
+      <c r="M28" s="64">
         <f>AVERAGE(I4:I28)</f>
         <v>91.600245901639354</v>
       </c>
-      <c r="N28" s="70">
+      <c r="N28" s="65">
         <f>SUM(H4:H28)</f>
         <v>4470</v>
       </c>
-      <c r="O28" s="69">
+      <c r="O28" s="64">
         <f>MAX(I4:I28)</f>
         <v>95.901639344262293</v>
       </c>
-      <c r="P28" s="71">
+      <c r="P28" s="66">
         <f>MIN(I4:I28)</f>
         <v>69.3</v>
       </c>
     </row>
-    <row r="29" spans="2:16">
-      <c r="B29" s="84" t="s">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B29" s="78" t="s">
         <v>179</v>
       </c>
       <c r="C29" s="44">
@@ -2472,13 +2489,13 @@
       <c r="J29" s="46"/>
       <c r="K29" s="46"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="62"/>
+      <c r="M29" s="57"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="63"/>
-    </row>
-    <row r="30" spans="2:16">
-      <c r="B30" s="89"/>
+      <c r="P29" s="58"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B30" s="83"/>
       <c r="C30" s="42">
         <v>27</v>
       </c>
@@ -2502,13 +2519,13 @@
       <c r="J30" s="47"/>
       <c r="K30" s="47"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="62"/>
+      <c r="M30" s="57"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="63"/>
-    </row>
-    <row r="31" spans="2:16">
-      <c r="B31" s="89"/>
+      <c r="P30" s="58"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B31" s="83"/>
       <c r="C31" s="42">
         <v>28</v>
       </c>
@@ -2532,13 +2549,13 @@
       <c r="J31" s="47"/>
       <c r="K31" s="47"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="62"/>
+      <c r="M31" s="57"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="63"/>
-    </row>
-    <row r="32" spans="2:16">
-      <c r="B32" s="89"/>
+      <c r="P31" s="58"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B32" s="83"/>
       <c r="C32" s="42">
         <v>29</v>
       </c>
@@ -2562,13 +2579,13 @@
       <c r="J32" s="47"/>
       <c r="K32" s="47"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="62"/>
+      <c r="M32" s="57"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="63"/>
-    </row>
-    <row r="33" spans="2:16">
-      <c r="B33" s="89"/>
+      <c r="P32" s="58"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B33" s="83"/>
       <c r="C33" s="42">
         <v>30</v>
       </c>
@@ -2592,13 +2609,13 @@
       <c r="J33" s="47"/>
       <c r="K33" s="47"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="62"/>
+      <c r="M33" s="57"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="63"/>
-    </row>
-    <row r="34" spans="2:16">
-      <c r="B34" s="89"/>
+      <c r="P33" s="58"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B34" s="83"/>
       <c r="C34" s="42">
         <v>31</v>
       </c>
@@ -2622,13 +2639,13 @@
       <c r="J34" s="47"/>
       <c r="K34" s="47"/>
       <c r="L34" s="1"/>
-      <c r="M34" s="62"/>
+      <c r="M34" s="57"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="63"/>
-    </row>
-    <row r="35" spans="2:16">
-      <c r="B35" s="89"/>
+      <c r="P34" s="58"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B35" s="83"/>
       <c r="C35" s="42">
         <v>32</v>
       </c>
@@ -2652,13 +2669,13 @@
       <c r="J35" s="47"/>
       <c r="K35" s="47"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="62"/>
+      <c r="M35" s="57"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="63"/>
-    </row>
-    <row r="36" spans="2:16">
-      <c r="B36" s="89"/>
+      <c r="P35" s="58"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B36" s="83"/>
       <c r="C36" s="42">
         <v>33</v>
       </c>
@@ -2682,13 +2699,13 @@
       <c r="J36" s="47"/>
       <c r="K36" s="47"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="62"/>
+      <c r="M36" s="57"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
-      <c r="P36" s="63"/>
-    </row>
-    <row r="37" spans="2:16">
-      <c r="B37" s="89"/>
+      <c r="P36" s="58"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B37" s="83"/>
       <c r="C37" s="42">
         <v>34</v>
       </c>
@@ -2712,13 +2729,13 @@
       <c r="J37" s="47"/>
       <c r="K37" s="47"/>
       <c r="L37" s="1"/>
-      <c r="M37" s="62"/>
+      <c r="M37" s="57"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="63"/>
-    </row>
-    <row r="38" spans="2:16">
-      <c r="B38" s="89"/>
+      <c r="P37" s="58"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B38" s="83"/>
       <c r="C38" s="42">
         <v>35</v>
       </c>
@@ -2742,13 +2759,13 @@
       <c r="J38" s="47"/>
       <c r="K38" s="47"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="62"/>
+      <c r="M38" s="57"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="63"/>
-    </row>
-    <row r="39" spans="2:16">
-      <c r="B39" s="89"/>
+      <c r="P38" s="58"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B39" s="83"/>
       <c r="C39" s="42">
         <v>36</v>
       </c>
@@ -2772,13 +2789,13 @@
       <c r="J39" s="47"/>
       <c r="K39" s="47"/>
       <c r="L39" s="1"/>
-      <c r="M39" s="62"/>
+      <c r="M39" s="57"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
-      <c r="P39" s="63"/>
-    </row>
-    <row r="40" spans="2:16">
-      <c r="B40" s="89"/>
+      <c r="P39" s="58"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B40" s="83"/>
       <c r="C40" s="42">
         <v>37</v>
       </c>
@@ -2804,13 +2821,13 @@
       <c r="L40" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="M40" s="62"/>
+      <c r="M40" s="57"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
-      <c r="P40" s="63"/>
-    </row>
-    <row r="41" spans="2:16">
-      <c r="B41" s="89"/>
+      <c r="P40" s="58"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B41" s="83"/>
       <c r="C41" s="42">
         <v>38</v>
       </c>
@@ -2834,13 +2851,13 @@
       <c r="J41" s="47"/>
       <c r="K41" s="47"/>
       <c r="L41" s="1"/>
-      <c r="M41" s="62"/>
+      <c r="M41" s="57"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
-      <c r="P41" s="63"/>
-    </row>
-    <row r="42" spans="2:16">
-      <c r="B42" s="89"/>
+      <c r="P41" s="58"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B42" s="83"/>
       <c r="C42" s="42">
         <v>39</v>
       </c>
@@ -2864,13 +2881,13 @@
       <c r="J42" s="47"/>
       <c r="K42" s="47"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="62"/>
+      <c r="M42" s="57"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
-      <c r="P42" s="63"/>
-    </row>
-    <row r="43" spans="2:16">
-      <c r="B43" s="89"/>
+      <c r="P42" s="58"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B43" s="83"/>
       <c r="C43" s="42">
         <v>40</v>
       </c>
@@ -2894,13 +2911,13 @@
       <c r="J43" s="47"/>
       <c r="K43" s="47"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="62"/>
+      <c r="M43" s="57"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
-      <c r="P43" s="63"/>
-    </row>
-    <row r="44" spans="2:16">
-      <c r="B44" s="89"/>
+      <c r="P43" s="58"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B44" s="83"/>
       <c r="C44" s="42">
         <v>41</v>
       </c>
@@ -2924,13 +2941,13 @@
       <c r="J44" s="47"/>
       <c r="K44" s="47"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="62"/>
+      <c r="M44" s="57"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
-      <c r="P44" s="63"/>
-    </row>
-    <row r="45" spans="2:16">
-      <c r="B45" s="89"/>
+      <c r="P44" s="58"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B45" s="83"/>
       <c r="C45" s="42">
         <v>42</v>
       </c>
@@ -2954,13 +2971,13 @@
       <c r="J45" s="47"/>
       <c r="K45" s="47"/>
       <c r="L45" s="1"/>
-      <c r="M45" s="62"/>
+      <c r="M45" s="57"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
-      <c r="P45" s="63"/>
-    </row>
-    <row r="46" spans="2:16">
-      <c r="B46" s="89"/>
+      <c r="P45" s="58"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B46" s="83"/>
       <c r="C46" s="42">
         <v>43</v>
       </c>
@@ -2984,13 +3001,13 @@
       <c r="J46" s="47"/>
       <c r="K46" s="47"/>
       <c r="L46" s="1"/>
-      <c r="M46" s="62"/>
+      <c r="M46" s="57"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
-      <c r="P46" s="63"/>
-    </row>
-    <row r="47" spans="2:16">
-      <c r="B47" s="89"/>
+      <c r="P46" s="58"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B47" s="83"/>
       <c r="C47" s="42">
         <v>44</v>
       </c>
@@ -3014,13 +3031,13 @@
       <c r="J47" s="47"/>
       <c r="K47" s="47"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="62"/>
+      <c r="M47" s="57"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
-      <c r="P47" s="63"/>
-    </row>
-    <row r="48" spans="2:16">
-      <c r="B48" s="89"/>
+      <c r="P47" s="58"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B48" s="83"/>
       <c r="C48" s="42">
         <v>45</v>
       </c>
@@ -3044,13 +3061,13 @@
       <c r="J48" s="47"/>
       <c r="K48" s="47"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="62"/>
+      <c r="M48" s="57"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="63"/>
-    </row>
-    <row r="49" spans="2:16">
-      <c r="B49" s="89"/>
+      <c r="P48" s="58"/>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B49" s="83"/>
       <c r="C49" s="42">
         <v>46</v>
       </c>
@@ -3074,13 +3091,13 @@
       <c r="J49" s="47"/>
       <c r="K49" s="47"/>
       <c r="L49" s="1"/>
-      <c r="M49" s="62"/>
+      <c r="M49" s="57"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-      <c r="P49" s="63"/>
-    </row>
-    <row r="50" spans="2:16">
-      <c r="B50" s="89"/>
+      <c r="P49" s="58"/>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B50" s="83"/>
       <c r="C50" s="42">
         <v>47</v>
       </c>
@@ -3104,13 +3121,13 @@
       <c r="J50" s="47"/>
       <c r="K50" s="47"/>
       <c r="L50" s="1"/>
-      <c r="M50" s="64"/>
-      <c r="N50" s="68"/>
+      <c r="M50" s="59"/>
+      <c r="N50" s="63"/>
       <c r="O50" s="1"/>
-      <c r="P50" s="63"/>
-    </row>
-    <row r="51" spans="2:16">
-      <c r="B51" s="90"/>
+      <c r="P50" s="58"/>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B51" s="84"/>
       <c r="C51" s="48">
         <v>48</v>
       </c>
@@ -3134,25 +3151,25 @@
       <c r="J51" s="51"/>
       <c r="K51" s="51"/>
       <c r="L51" s="2"/>
-      <c r="M51" s="69">
+      <c r="M51" s="64">
         <f>AVERAGE(I29:I51)</f>
         <v>92.640769779044902</v>
       </c>
-      <c r="N51" s="70">
+      <c r="N51" s="65">
         <f>SUM(H29:H51)</f>
         <v>5199</v>
       </c>
-      <c r="O51" s="69">
+      <c r="O51" s="64">
         <f>MAX(I29:I51)</f>
         <v>96.311475409836063</v>
       </c>
-      <c r="P51" s="71">
+      <c r="P51" s="66">
         <f>MIN(I29:I51)</f>
         <v>81.147540983606561</v>
       </c>
     </row>
-    <row r="52" spans="2:16">
-      <c r="B52" s="84" t="s">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B52" s="78" t="s">
         <v>208</v>
       </c>
       <c r="C52" s="44">
@@ -3179,13 +3196,13 @@
       <c r="L52" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="M52" s="62"/>
+      <c r="M52" s="57"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
-      <c r="P52" s="63"/>
-    </row>
-    <row r="53" spans="2:16">
-      <c r="B53" s="90"/>
+      <c r="P52" s="58"/>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B53" s="84"/>
       <c r="C53" s="48">
         <v>50</v>
       </c>
@@ -3210,25 +3227,25 @@
       <c r="L53" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="M53" s="69">
+      <c r="M53" s="64">
         <f>AVERAGE(I52:I53)</f>
         <v>93.05</v>
       </c>
-      <c r="N53" s="70">
+      <c r="N53" s="65">
         <f>SUM(H52:H53)</f>
         <v>454</v>
       </c>
-      <c r="O53" s="69">
+      <c r="O53" s="64">
         <f>MAX(I52:I53)</f>
         <v>96.3</v>
       </c>
-      <c r="P53" s="71">
+      <c r="P53" s="66">
         <f>MIN(I52:I53)</f>
         <v>89.8</v>
       </c>
     </row>
-    <row r="54" spans="2:16">
-      <c r="B54" s="84" t="s">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B54" s="78" t="s">
         <v>172</v>
       </c>
       <c r="C54" s="44">
@@ -3251,13 +3268,13 @@
       <c r="J54" s="46"/>
       <c r="K54" s="46"/>
       <c r="L54" s="3"/>
-      <c r="M54" s="62"/>
+      <c r="M54" s="57"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
-      <c r="P54" s="63"/>
-    </row>
-    <row r="55" spans="2:16">
-      <c r="B55" s="85"/>
+      <c r="P54" s="58"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B55" s="79"/>
       <c r="C55" s="42">
         <v>52</v>
       </c>
@@ -3278,13 +3295,13 @@
       <c r="J55" s="47"/>
       <c r="K55" s="47"/>
       <c r="L55" s="1"/>
-      <c r="M55" s="62"/>
+      <c r="M55" s="57"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
-      <c r="P55" s="63"/>
-    </row>
-    <row r="56" spans="2:16">
-      <c r="B56" s="85"/>
+      <c r="P55" s="58"/>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B56" s="79"/>
       <c r="C56" s="42">
         <v>53</v>
       </c>
@@ -3305,13 +3322,13 @@
       <c r="J56" s="47"/>
       <c r="K56" s="47"/>
       <c r="L56" s="1"/>
-      <c r="M56" s="62"/>
+      <c r="M56" s="57"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
-      <c r="P56" s="63"/>
-    </row>
-    <row r="57" spans="2:16">
-      <c r="B57" s="85"/>
+      <c r="P56" s="58"/>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B57" s="79"/>
       <c r="C57" s="42">
         <v>54</v>
       </c>
@@ -3332,13 +3349,13 @@
       <c r="J57" s="47"/>
       <c r="K57" s="47"/>
       <c r="L57" s="1"/>
-      <c r="M57" s="62"/>
+      <c r="M57" s="57"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
-      <c r="P57" s="63"/>
-    </row>
-    <row r="58" spans="2:16">
-      <c r="B58" s="85"/>
+      <c r="P57" s="58"/>
+    </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B58" s="79"/>
       <c r="C58" s="42">
         <v>55</v>
       </c>
@@ -3359,13 +3376,13 @@
       <c r="J58" s="47"/>
       <c r="K58" s="47"/>
       <c r="L58" s="1"/>
-      <c r="M58" s="62"/>
+      <c r="M58" s="57"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
-      <c r="P58" s="63"/>
-    </row>
-    <row r="59" spans="2:16">
-      <c r="B59" s="85"/>
+      <c r="P58" s="58"/>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B59" s="79"/>
       <c r="C59" s="42">
         <v>56</v>
       </c>
@@ -3386,13 +3403,13 @@
       <c r="J59" s="47"/>
       <c r="K59" s="47"/>
       <c r="L59" s="1"/>
-      <c r="M59" s="62"/>
+      <c r="M59" s="57"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
-      <c r="P59" s="63"/>
-    </row>
-    <row r="60" spans="2:16">
-      <c r="B60" s="85"/>
+      <c r="P59" s="58"/>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B60" s="79"/>
       <c r="C60" s="42">
         <v>57</v>
       </c>
@@ -3413,13 +3430,13 @@
       <c r="J60" s="47"/>
       <c r="K60" s="47"/>
       <c r="L60" s="1"/>
-      <c r="M60" s="62"/>
+      <c r="M60" s="57"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
-      <c r="P60" s="63"/>
-    </row>
-    <row r="61" spans="2:16">
-      <c r="B61" s="85"/>
+      <c r="P60" s="58"/>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B61" s="79"/>
       <c r="C61" s="42">
         <v>58</v>
       </c>
@@ -3440,13 +3457,13 @@
       <c r="J61" s="47"/>
       <c r="K61" s="47"/>
       <c r="L61" s="1"/>
-      <c r="M61" s="62"/>
+      <c r="M61" s="57"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
-      <c r="P61" s="63"/>
-    </row>
-    <row r="62" spans="2:16">
-      <c r="B62" s="85"/>
+      <c r="P61" s="58"/>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B62" s="79"/>
       <c r="C62" s="42">
         <v>59</v>
       </c>
@@ -3467,13 +3484,13 @@
       <c r="J62" s="47"/>
       <c r="K62" s="47"/>
       <c r="L62" s="1"/>
-      <c r="M62" s="62"/>
+      <c r="M62" s="57"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
-      <c r="P62" s="63"/>
-    </row>
-    <row r="63" spans="2:16">
-      <c r="B63" s="85"/>
+      <c r="P62" s="58"/>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B63" s="79"/>
       <c r="C63" s="42">
         <v>60</v>
       </c>
@@ -3494,13 +3511,13 @@
       <c r="J63" s="47"/>
       <c r="K63" s="47"/>
       <c r="L63" s="1"/>
-      <c r="M63" s="62"/>
+      <c r="M63" s="57"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
-      <c r="P63" s="63"/>
-    </row>
-    <row r="64" spans="2:16">
-      <c r="B64" s="85"/>
+      <c r="P63" s="58"/>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B64" s="79"/>
       <c r="C64" s="42">
         <v>61</v>
       </c>
@@ -3521,13 +3538,13 @@
       <c r="J64" s="47"/>
       <c r="K64" s="47"/>
       <c r="L64" s="1"/>
-      <c r="M64" s="62"/>
+      <c r="M64" s="57"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
-      <c r="P64" s="63"/>
-    </row>
-    <row r="65" spans="2:16">
-      <c r="B65" s="85"/>
+      <c r="P64" s="58"/>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B65" s="79"/>
       <c r="C65" s="42">
         <v>62</v>
       </c>
@@ -3548,13 +3565,13 @@
       <c r="J65" s="47"/>
       <c r="K65" s="47"/>
       <c r="L65" s="1"/>
-      <c r="M65" s="62"/>
+      <c r="M65" s="57"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
-      <c r="P65" s="63"/>
-    </row>
-    <row r="66" spans="2:16">
-      <c r="B66" s="85"/>
+      <c r="P65" s="58"/>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B66" s="79"/>
       <c r="C66" s="42">
         <v>63</v>
       </c>
@@ -3575,13 +3592,13 @@
       <c r="J66" s="47"/>
       <c r="K66" s="47"/>
       <c r="L66" s="1"/>
-      <c r="M66" s="62"/>
+      <c r="M66" s="57"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
-      <c r="P66" s="63"/>
-    </row>
-    <row r="67" spans="2:16">
-      <c r="B67" s="85"/>
+      <c r="P66" s="58"/>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B67" s="79"/>
       <c r="C67" s="42">
         <v>64</v>
       </c>
@@ -3602,13 +3619,13 @@
       <c r="J67" s="47"/>
       <c r="K67" s="47"/>
       <c r="L67" s="1"/>
-      <c r="M67" s="62"/>
+      <c r="M67" s="57"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
-      <c r="P67" s="63"/>
-    </row>
-    <row r="68" spans="2:16">
-      <c r="B68" s="85"/>
+      <c r="P67" s="58"/>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B68" s="79"/>
       <c r="C68" s="42">
         <v>65</v>
       </c>
@@ -3629,13 +3646,13 @@
       <c r="J68" s="47"/>
       <c r="K68" s="47"/>
       <c r="L68" s="1"/>
-      <c r="M68" s="62"/>
+      <c r="M68" s="57"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
-      <c r="P68" s="63"/>
-    </row>
-    <row r="69" spans="2:16">
-      <c r="B69" s="85"/>
+      <c r="P68" s="58"/>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B69" s="79"/>
       <c r="C69" s="42">
         <v>66</v>
       </c>
@@ -3656,13 +3673,13 @@
       <c r="J69" s="47"/>
       <c r="K69" s="47"/>
       <c r="L69" s="1"/>
-      <c r="M69" s="62"/>
+      <c r="M69" s="57"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
-      <c r="P69" s="63"/>
-    </row>
-    <row r="70" spans="2:16">
-      <c r="B70" s="85"/>
+      <c r="P69" s="58"/>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B70" s="79"/>
       <c r="C70" s="42">
         <v>67</v>
       </c>
@@ -3683,13 +3700,13 @@
       <c r="J70" s="47"/>
       <c r="K70" s="47"/>
       <c r="L70" s="1"/>
-      <c r="M70" s="62"/>
+      <c r="M70" s="57"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
-      <c r="P70" s="63"/>
-    </row>
-    <row r="71" spans="2:16">
-      <c r="B71" s="85"/>
+      <c r="P70" s="58"/>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B71" s="79"/>
       <c r="C71" s="42">
         <v>68</v>
       </c>
@@ -3709,14 +3726,14 @@
       </c>
       <c r="J71" s="47"/>
       <c r="K71" s="47"/>
-      <c r="L71" s="72"/>
-      <c r="M71" s="62"/>
+      <c r="L71" s="67"/>
+      <c r="M71" s="57"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
-      <c r="P71" s="63"/>
-    </row>
-    <row r="72" spans="2:16">
-      <c r="B72" s="85"/>
+      <c r="P71" s="58"/>
+    </row>
+    <row r="72" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B72" s="79"/>
       <c r="C72" s="42">
         <v>69</v>
       </c>
@@ -3736,16 +3753,16 @@
       </c>
       <c r="J72" s="47"/>
       <c r="K72" s="47"/>
-      <c r="L72" s="72" t="s">
+      <c r="L72" s="67" t="s">
         <v>262</v>
       </c>
-      <c r="M72" s="62"/>
+      <c r="M72" s="57"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
-      <c r="P72" s="63"/>
-    </row>
-    <row r="73" spans="2:16">
-      <c r="B73" s="85"/>
+      <c r="P72" s="58"/>
+    </row>
+    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B73" s="79"/>
       <c r="C73" s="42">
         <v>70</v>
       </c>
@@ -3765,16 +3782,16 @@
       </c>
       <c r="J73" s="47"/>
       <c r="K73" s="47"/>
-      <c r="L73" s="73" t="s">
+      <c r="L73" s="68" t="s">
         <v>272</v>
       </c>
-      <c r="M73" s="62"/>
+      <c r="M73" s="57"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
-      <c r="P73" s="63"/>
-    </row>
-    <row r="74" spans="2:16">
-      <c r="B74" s="85"/>
+      <c r="P73" s="58"/>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B74" s="79"/>
       <c r="C74" s="42">
         <v>71</v>
       </c>
@@ -3794,14 +3811,14 @@
       </c>
       <c r="J74" s="47"/>
       <c r="K74" s="47"/>
-      <c r="L74" s="72"/>
-      <c r="M74" s="62"/>
+      <c r="L74" s="67"/>
+      <c r="M74" s="57"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
-      <c r="P74" s="63"/>
-    </row>
-    <row r="75" spans="2:16">
-      <c r="B75" s="85"/>
+      <c r="P74" s="58"/>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B75" s="79"/>
       <c r="C75" s="42">
         <v>72</v>
       </c>
@@ -3821,14 +3838,14 @@
       </c>
       <c r="J75" s="47"/>
       <c r="K75" s="47"/>
-      <c r="L75" s="72"/>
-      <c r="M75" s="62"/>
+      <c r="L75" s="67"/>
+      <c r="M75" s="57"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
-      <c r="P75" s="63"/>
-    </row>
-    <row r="76" spans="2:16">
-      <c r="B76" s="85"/>
+      <c r="P75" s="58"/>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B76" s="79"/>
       <c r="C76" s="42">
         <v>73</v>
       </c>
@@ -3848,14 +3865,14 @@
       </c>
       <c r="J76" s="47"/>
       <c r="K76" s="47"/>
-      <c r="L76" s="72"/>
-      <c r="M76" s="62"/>
+      <c r="L76" s="67"/>
+      <c r="M76" s="57"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
-      <c r="P76" s="63"/>
-    </row>
-    <row r="77" spans="2:16">
-      <c r="B77" s="85"/>
+      <c r="P76" s="58"/>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B77" s="79"/>
       <c r="C77" s="42">
         <v>74</v>
       </c>
@@ -3875,14 +3892,14 @@
       </c>
       <c r="J77" s="47"/>
       <c r="K77" s="47"/>
-      <c r="L77" s="72"/>
-      <c r="M77" s="64"/>
-      <c r="N77" s="68"/>
+      <c r="L77" s="67"/>
+      <c r="M77" s="59"/>
+      <c r="N77" s="63"/>
       <c r="O77" s="1"/>
-      <c r="P77" s="63"/>
-    </row>
-    <row r="78" spans="2:16">
-      <c r="B78" s="86"/>
+      <c r="P77" s="58"/>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B78" s="80"/>
       <c r="C78" s="48">
         <v>75</v>
       </c>
@@ -3902,28 +3919,28 @@
       </c>
       <c r="J78" s="51"/>
       <c r="K78" s="51"/>
-      <c r="L78" s="74" t="s">
+      <c r="L78" s="69" t="s">
         <v>263</v>
       </c>
-      <c r="M78" s="69">
+      <c r="M78" s="64">
         <f>AVERAGE(I54:I78)</f>
         <v>93.531999999999982</v>
       </c>
-      <c r="N78" s="70">
+      <c r="N78" s="65">
         <f>SUM(H54:H78)</f>
         <v>5705</v>
       </c>
-      <c r="O78" s="69">
+      <c r="O78" s="64">
         <f>MAX(I54:I78)</f>
         <v>97.1</v>
       </c>
-      <c r="P78" s="71">
+      <c r="P78" s="66">
         <f>MIN(I54:I78)</f>
         <v>88.9</v>
       </c>
     </row>
-    <row r="79" spans="2:16" ht="12.75" customHeight="1">
-      <c r="B79" s="84" t="s">
+    <row r="79" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="78" t="s">
         <v>172</v>
       </c>
       <c r="C79" s="44">
@@ -3945,14 +3962,14 @@
       </c>
       <c r="J79" s="46"/>
       <c r="K79" s="46"/>
-      <c r="L79" s="75"/>
-      <c r="M79" s="62"/>
+      <c r="L79" s="70"/>
+      <c r="M79" s="57"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
-      <c r="P79" s="63"/>
-    </row>
-    <row r="80" spans="2:16">
-      <c r="B80" s="85"/>
+      <c r="P79" s="58"/>
+    </row>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B80" s="79"/>
       <c r="C80" s="42">
         <v>77</v>
       </c>
@@ -3972,16 +3989,16 @@
       </c>
       <c r="J80" s="47"/>
       <c r="K80" s="47"/>
-      <c r="L80" s="72" t="s">
+      <c r="L80" s="67" t="s">
         <v>273</v>
       </c>
-      <c r="M80" s="62"/>
+      <c r="M80" s="57"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
-      <c r="P80" s="63"/>
-    </row>
-    <row r="81" spans="2:16">
-      <c r="B81" s="85"/>
+      <c r="P80" s="58"/>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B81" s="79"/>
       <c r="C81" s="42">
         <v>78</v>
       </c>
@@ -4002,13 +4019,13 @@
       <c r="J81" s="47"/>
       <c r="K81" s="47"/>
       <c r="L81" s="1"/>
-      <c r="M81" s="62"/>
+      <c r="M81" s="57"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
-      <c r="P81" s="63"/>
-    </row>
-    <row r="82" spans="2:16">
-      <c r="B82" s="85"/>
+      <c r="P81" s="58"/>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B82" s="79"/>
       <c r="C82" s="42">
         <v>79</v>
       </c>
@@ -4029,13 +4046,13 @@
       <c r="J82" s="47"/>
       <c r="K82" s="47"/>
       <c r="L82" s="1"/>
-      <c r="M82" s="62"/>
+      <c r="M82" s="57"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
-      <c r="P82" s="63"/>
-    </row>
-    <row r="83" spans="2:16">
-      <c r="B83" s="85"/>
+      <c r="P82" s="58"/>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B83" s="79"/>
       <c r="C83" s="42">
         <v>80</v>
       </c>
@@ -4056,13 +4073,13 @@
       <c r="J83" s="47"/>
       <c r="K83" s="47"/>
       <c r="L83" s="1"/>
-      <c r="M83" s="62"/>
+      <c r="M83" s="57"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
-      <c r="P83" s="63"/>
-    </row>
-    <row r="84" spans="2:16">
-      <c r="B84" s="85"/>
+      <c r="P83" s="58"/>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B84" s="79"/>
       <c r="C84" s="42">
         <v>81</v>
       </c>
@@ -4083,13 +4100,13 @@
       <c r="J84" s="47"/>
       <c r="K84" s="47"/>
       <c r="L84" s="1"/>
-      <c r="M84" s="62"/>
+      <c r="M84" s="57"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
-      <c r="P84" s="63"/>
-    </row>
-    <row r="85" spans="2:16">
-      <c r="B85" s="85"/>
+      <c r="P84" s="58"/>
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B85" s="79"/>
       <c r="C85" s="42">
         <v>82</v>
       </c>
@@ -4110,13 +4127,13 @@
       <c r="J85" s="47"/>
       <c r="K85" s="47"/>
       <c r="L85" s="1"/>
-      <c r="M85" s="62"/>
+      <c r="M85" s="57"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
-      <c r="P85" s="63"/>
-    </row>
-    <row r="86" spans="2:16">
-      <c r="B86" s="85"/>
+      <c r="P85" s="58"/>
+    </row>
+    <row r="86" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B86" s="79"/>
       <c r="C86" s="42">
         <v>83</v>
       </c>
@@ -4137,13 +4154,13 @@
       <c r="J86" s="47"/>
       <c r="K86" s="47"/>
       <c r="L86" s="1"/>
-      <c r="M86" s="62"/>
+      <c r="M86" s="57"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
-      <c r="P86" s="63"/>
-    </row>
-    <row r="87" spans="2:16">
-      <c r="B87" s="85"/>
+      <c r="P86" s="58"/>
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B87" s="79"/>
       <c r="C87" s="42">
         <v>84</v>
       </c>
@@ -4166,13 +4183,13 @@
       <c r="L87" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="M87" s="62"/>
+      <c r="M87" s="57"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
-      <c r="P87" s="63"/>
-    </row>
-    <row r="88" spans="2:16">
-      <c r="B88" s="85"/>
+      <c r="P87" s="58"/>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B88" s="79"/>
       <c r="C88" s="42">
         <v>85</v>
       </c>
@@ -4193,13 +4210,13 @@
       <c r="J88" s="47"/>
       <c r="K88" s="47"/>
       <c r="L88" s="1"/>
-      <c r="M88" s="62"/>
+      <c r="M88" s="57"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
-      <c r="P88" s="63"/>
-    </row>
-    <row r="89" spans="2:16">
-      <c r="B89" s="85"/>
+      <c r="P88" s="58"/>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B89" s="79"/>
       <c r="C89" s="42">
         <v>86</v>
       </c>
@@ -4222,13 +4239,13 @@
       <c r="L89" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="M89" s="62"/>
+      <c r="M89" s="57"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
-      <c r="P89" s="63"/>
-    </row>
-    <row r="90" spans="2:16">
-      <c r="B90" s="85"/>
+      <c r="P89" s="58"/>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B90" s="79"/>
       <c r="C90" s="42">
         <v>87</v>
       </c>
@@ -4251,13 +4268,13 @@
       <c r="L90" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="M90" s="62"/>
+      <c r="M90" s="57"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
-      <c r="P90" s="63"/>
-    </row>
-    <row r="91" spans="2:16">
-      <c r="B91" s="85"/>
+      <c r="P90" s="58"/>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B91" s="79"/>
       <c r="C91" s="42">
         <v>88</v>
       </c>
@@ -4278,13 +4295,13 @@
       <c r="J91" s="47"/>
       <c r="K91" s="47"/>
       <c r="L91" s="1"/>
-      <c r="M91" s="62"/>
+      <c r="M91" s="57"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
-      <c r="P91" s="63"/>
-    </row>
-    <row r="92" spans="2:16">
-      <c r="B92" s="85"/>
+      <c r="P91" s="58"/>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B92" s="79"/>
       <c r="C92" s="42">
         <v>89</v>
       </c>
@@ -4305,13 +4322,13 @@
       <c r="J92" s="47"/>
       <c r="K92" s="47"/>
       <c r="L92" s="1"/>
-      <c r="M92" s="62"/>
+      <c r="M92" s="57"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
-      <c r="P92" s="63"/>
-    </row>
-    <row r="93" spans="2:16">
-      <c r="B93" s="85"/>
+      <c r="P92" s="58"/>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B93" s="79"/>
       <c r="C93" s="42">
         <v>90</v>
       </c>
@@ -4332,13 +4349,13 @@
       <c r="J93" s="47"/>
       <c r="K93" s="47"/>
       <c r="L93" s="1"/>
-      <c r="M93" s="62"/>
+      <c r="M93" s="57"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
-      <c r="P93" s="63"/>
-    </row>
-    <row r="94" spans="2:16">
-      <c r="B94" s="85"/>
+      <c r="P93" s="58"/>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B94" s="79"/>
       <c r="C94" s="42">
         <v>91</v>
       </c>
@@ -4359,13 +4376,13 @@
       <c r="J94" s="47"/>
       <c r="K94" s="47"/>
       <c r="L94" s="1"/>
-      <c r="M94" s="62"/>
+      <c r="M94" s="57"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
-      <c r="P94" s="63"/>
-    </row>
-    <row r="95" spans="2:16">
-      <c r="B95" s="85"/>
+      <c r="P94" s="58"/>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B95" s="79"/>
       <c r="C95" s="42">
         <v>92</v>
       </c>
@@ -4386,13 +4403,13 @@
       <c r="J95" s="47"/>
       <c r="K95" s="47"/>
       <c r="L95" s="1"/>
-      <c r="M95" s="62"/>
+      <c r="M95" s="57"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
-      <c r="P95" s="63"/>
-    </row>
-    <row r="96" spans="2:16">
-      <c r="B96" s="85"/>
+      <c r="P95" s="58"/>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B96" s="79"/>
       <c r="C96" s="42">
         <v>93</v>
       </c>
@@ -4415,13 +4432,13 @@
       <c r="L96" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="M96" s="62"/>
+      <c r="M96" s="57"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
-      <c r="P96" s="63"/>
-    </row>
-    <row r="97" spans="2:16">
-      <c r="B97" s="85"/>
+      <c r="P96" s="58"/>
+    </row>
+    <row r="97" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B97" s="79"/>
       <c r="C97" s="42">
         <v>94</v>
       </c>
@@ -4444,13 +4461,13 @@
       <c r="L97" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="M97" s="62"/>
+      <c r="M97" s="57"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
-      <c r="P97" s="63"/>
-    </row>
-    <row r="98" spans="2:16">
-      <c r="B98" s="85"/>
+      <c r="P97" s="58"/>
+    </row>
+    <row r="98" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B98" s="79"/>
       <c r="C98" s="42">
         <v>95</v>
       </c>
@@ -4473,13 +4490,13 @@
       <c r="L98" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="M98" s="62"/>
+      <c r="M98" s="57"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
-      <c r="P98" s="63"/>
-    </row>
-    <row r="99" spans="2:16">
-      <c r="B99" s="85"/>
+      <c r="P98" s="58"/>
+    </row>
+    <row r="99" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B99" s="79"/>
       <c r="C99" s="42">
         <v>96</v>
       </c>
@@ -4502,13 +4519,13 @@
       <c r="L99" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="M99" s="62"/>
+      <c r="M99" s="57"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
-      <c r="P99" s="63"/>
-    </row>
-    <row r="100" spans="2:16">
-      <c r="B100" s="85"/>
+      <c r="P99" s="58"/>
+    </row>
+    <row r="100" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B100" s="79"/>
       <c r="C100" s="42">
         <v>97</v>
       </c>
@@ -4529,20 +4546,20 @@
       <c r="J100" s="47"/>
       <c r="K100" s="47"/>
       <c r="L100" s="1"/>
-      <c r="M100" s="62"/>
+      <c r="M100" s="57"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
-      <c r="P100" s="63"/>
-    </row>
-    <row r="101" spans="2:16">
-      <c r="B101" s="85"/>
+      <c r="P100" s="58"/>
+    </row>
+    <row r="101" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B101" s="79"/>
       <c r="C101" s="42">
         <v>98</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E101" s="56" t="s">
+      <c r="E101" s="53" t="s">
         <v>265</v>
       </c>
       <c r="F101" s="1"/>
@@ -4553,18 +4570,18 @@
       <c r="I101" s="11">
         <v>92.6</v>
       </c>
-      <c r="J101" s="57"/>
+      <c r="J101" s="54"/>
       <c r="K101" s="47"/>
-      <c r="L101" s="57" t="s">
+      <c r="L101" s="54" t="s">
         <v>281</v>
       </c>
-      <c r="M101" s="62"/>
+      <c r="M101" s="57"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
-      <c r="P101" s="63"/>
-    </row>
-    <row r="102" spans="2:16">
-      <c r="B102" s="85"/>
+      <c r="P101" s="58"/>
+    </row>
+    <row r="102" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B102" s="79"/>
       <c r="C102" s="42">
         <v>99</v>
       </c>
@@ -4583,13 +4600,13 @@
       <c r="L102" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="M102" s="62"/>
+      <c r="M102" s="57"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1"/>
-      <c r="P102" s="63"/>
-    </row>
-    <row r="103" spans="2:16">
-      <c r="B103" s="85"/>
+      <c r="P102" s="58"/>
+    </row>
+    <row r="103" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B103" s="79"/>
       <c r="C103" s="42">
         <v>100</v>
       </c>
@@ -4608,13 +4625,13 @@
       <c r="L103" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="M103" s="64"/>
-      <c r="N103" s="68"/>
+      <c r="M103" s="59"/>
+      <c r="N103" s="63"/>
       <c r="O103" s="1"/>
-      <c r="P103" s="63"/>
-    </row>
-    <row r="104" spans="2:16" ht="13.5" thickBot="1">
-      <c r="B104" s="86"/>
+      <c r="P103" s="58"/>
+    </row>
+    <row r="104" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B104" s="80"/>
       <c r="C104" s="48">
         <v>101</v>
       </c>
@@ -4633,317 +4650,371 @@
       <c r="L104" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M104" s="77">
+      <c r="M104" s="66">
         <f>AVERAGE(I79:I104)</f>
         <v>93.182608695652192</v>
       </c>
-      <c r="N104" s="78">
+      <c r="N104" s="65">
         <f>SUM(H79:H104)</f>
         <v>5229</v>
       </c>
-      <c r="O104" s="77">
+      <c r="O104" s="66">
         <f>MAX(I79:I104)</f>
         <v>98.8</v>
       </c>
-      <c r="P104" s="10">
+      <c r="P104" s="66">
         <f>MIN(I79:I104)</f>
         <v>88.9</v>
       </c>
     </row>
-    <row r="105" spans="2:16" ht="13.5" thickBot="1">
-      <c r="L105" s="76" t="s">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B105" s="78" t="s">
+        <v>283</v>
+      </c>
+      <c r="C105" s="44">
+        <v>102</v>
+      </c>
+      <c r="D105" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="E105" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="F105" s="3"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="46"/>
+      <c r="K105" s="46"/>
+      <c r="L105" s="70"/>
+      <c r="M105" s="57"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="58"/>
+    </row>
+    <row r="106" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B106" s="79"/>
+      <c r="C106" s="42">
+        <v>103</v>
+      </c>
+      <c r="D106" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E106" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="F106" s="1"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="11"/>
+      <c r="J106" s="47"/>
+      <c r="K106" s="47"/>
+      <c r="L106" s="67"/>
+      <c r="M106" s="57"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+      <c r="P106" s="58"/>
+    </row>
+    <row r="107" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B107" s="79"/>
+      <c r="C107" s="42">
+        <v>104</v>
+      </c>
+      <c r="D107" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E107" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="11"/>
+      <c r="J107" s="47"/>
+      <c r="K107" s="47"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="57"/>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1"/>
+      <c r="P107" s="58"/>
+    </row>
+    <row r="108" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B108" s="79"/>
+      <c r="C108" s="42">
+        <v>105</v>
+      </c>
+      <c r="D108" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E108" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="47"/>
+      <c r="K108" s="47"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="57"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+      <c r="P108" s="58"/>
+    </row>
+    <row r="109" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B109" s="79"/>
+      <c r="C109" s="42">
+        <v>106</v>
+      </c>
+      <c r="D109" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E109" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="47"/>
+      <c r="J109" s="47"/>
+      <c r="K109" s="47"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="57"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1"/>
+      <c r="P109" s="58"/>
+    </row>
+    <row r="110" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B110" s="79"/>
+      <c r="C110" s="42">
+        <v>107</v>
+      </c>
+      <c r="D110" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E110" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="11"/>
+      <c r="J110" s="47"/>
+      <c r="K110" s="47"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="57"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+      <c r="P110" s="58"/>
+    </row>
+    <row r="111" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B111" s="79"/>
+      <c r="C111" s="42">
+        <v>108</v>
+      </c>
+      <c r="D111" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E111" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="11"/>
+      <c r="J111" s="47"/>
+      <c r="K111" s="47"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="59"/>
+      <c r="N111" s="63"/>
+      <c r="O111" s="1"/>
+      <c r="P111" s="58"/>
+    </row>
+    <row r="112" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="80"/>
+      <c r="C112" s="48">
+        <v>109</v>
+      </c>
+      <c r="D112" s="49" t="s">
+        <v>284</v>
+      </c>
+      <c r="E112" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="50"/>
+      <c r="J112" s="51"/>
+      <c r="K112" s="51"/>
+      <c r="L112" s="2"/>
+      <c r="M112" s="72" t="e">
+        <f>AVERAGE(I105:I112)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N112" s="73">
+        <f>SUM(H105:H112)</f>
+        <v>0</v>
+      </c>
+      <c r="O112" s="72">
+        <f>MAX(I105:I112)</f>
+        <v>0</v>
+      </c>
+      <c r="P112" s="10">
+        <f>MIN(I105:I112)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L113" s="71" t="s">
         <v>267</v>
       </c>
-      <c r="M105" s="79">
-        <f>AVERAGE(M4:M104)</f>
-        <v>92.801124875267277</v>
-      </c>
-      <c r="N105" s="80">
-        <f>SUM(N4:N104)</f>
-        <v>21057</v>
-      </c>
-      <c r="O105" s="81">
-        <f>MAX(O4:O104)</f>
+      <c r="M113" s="74" t="e">
+        <f>AVERAGE(M30:M112)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N113" s="75">
+        <f>SUM(N30:N112)</f>
+        <v>16587</v>
+      </c>
+      <c r="O113" s="76">
+        <f>MAX(O30:O112)</f>
         <v>98.8</v>
       </c>
-      <c r="P105" s="82">
-        <f>MIN(P4:P104)</f>
-        <v>69.3</v>
-      </c>
-    </row>
-    <row r="106" spans="2:16">
-      <c r="C106" s="53"/>
-      <c r="D106" s="20"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="20"/>
-      <c r="G106" s="20"/>
-      <c r="H106" s="20"/>
-      <c r="I106" s="54"/>
-      <c r="J106" s="55"/>
-      <c r="K106" s="55"/>
-      <c r="L106" s="20"/>
-    </row>
-    <row r="107" spans="2:16">
-      <c r="C107" s="53"/>
-      <c r="D107" s="83"/>
-      <c r="E107" s="58"/>
-      <c r="F107" s="55"/>
-      <c r="G107" s="61"/>
-      <c r="H107" s="20"/>
-      <c r="I107" s="54"/>
-      <c r="J107" s="55"/>
-      <c r="K107" s="55"/>
-      <c r="L107" s="20"/>
-    </row>
-    <row r="108" spans="2:16">
-      <c r="E108" s="59"/>
-      <c r="F108" s="9"/>
-      <c r="G108" s="61"/>
-    </row>
-    <row r="109" spans="2:16">
-      <c r="E109" s="59"/>
-      <c r="F109" s="9"/>
-      <c r="G109" s="61"/>
-    </row>
-    <row r="110" spans="2:16">
-      <c r="E110" s="59"/>
-      <c r="F110" s="9"/>
-      <c r="G110" s="61"/>
-    </row>
-    <row r="111" spans="2:16">
-      <c r="E111" s="59"/>
-      <c r="F111" s="9"/>
-      <c r="G111" s="61"/>
-    </row>
-    <row r="112" spans="2:16">
-      <c r="E112" s="59"/>
-      <c r="F112" s="9"/>
-      <c r="G112" s="61"/>
-    </row>
-    <row r="113" spans="5:7">
-      <c r="E113" s="59"/>
-      <c r="F113" s="9"/>
-      <c r="G113" s="61"/>
-    </row>
-    <row r="114" spans="5:7">
-      <c r="E114" s="59"/>
+      <c r="P113" s="77">
+        <f>MIN(P30:P112)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="E114" s="55"/>
       <c r="F114" s="9"/>
-      <c r="G114" s="61"/>
-    </row>
-    <row r="115" spans="5:7">
-      <c r="E115" s="59"/>
+      <c r="G114" s="56"/>
+    </row>
+    <row r="115" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="E115" s="55"/>
       <c r="F115" s="9"/>
-      <c r="G115" s="61"/>
-    </row>
-    <row r="116" spans="5:7">
-      <c r="E116" s="59"/>
+      <c r="G115" s="56"/>
+    </row>
+    <row r="116" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="E116" s="55"/>
       <c r="F116" s="9"/>
-      <c r="G116" s="61"/>
-    </row>
-    <row r="117" spans="5:7">
-      <c r="E117" s="59"/>
+      <c r="G116" s="56"/>
+    </row>
+    <row r="117" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="E117" s="55"/>
       <c r="F117" s="9"/>
-      <c r="G117" s="61"/>
-    </row>
-    <row r="118" spans="5:7">
-      <c r="E118" s="59"/>
+      <c r="G117" s="56"/>
+    </row>
+    <row r="118" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="E118" s="55"/>
       <c r="F118" s="9"/>
-      <c r="G118" s="61"/>
-    </row>
-    <row r="119" spans="5:7">
-      <c r="E119" s="59"/>
-      <c r="F119" s="9"/>
-      <c r="G119" s="61"/>
-    </row>
-    <row r="120" spans="5:7">
-      <c r="E120" s="59"/>
-      <c r="F120" s="9"/>
-      <c r="G120" s="61"/>
-    </row>
-    <row r="121" spans="5:7">
-      <c r="E121" s="59"/>
-      <c r="F121" s="9"/>
-      <c r="G121" s="61"/>
-    </row>
-    <row r="122" spans="5:7">
-      <c r="E122" s="59"/>
-      <c r="F122" s="9"/>
-      <c r="G122" s="61"/>
-    </row>
-    <row r="123" spans="5:7">
-      <c r="E123" s="59"/>
-      <c r="F123" s="9"/>
-      <c r="G123" s="61"/>
-    </row>
-    <row r="124" spans="5:7">
-      <c r="E124" s="59"/>
-      <c r="F124" s="9"/>
-      <c r="G124" s="61"/>
-    </row>
-    <row r="125" spans="5:7">
-      <c r="E125" s="59"/>
-      <c r="F125" s="9"/>
-      <c r="G125" s="61"/>
-    </row>
-    <row r="126" spans="5:7">
-      <c r="E126" s="59"/>
-      <c r="F126" s="9"/>
-      <c r="G126" s="61"/>
-    </row>
-    <row r="127" spans="5:7">
-      <c r="E127" s="59"/>
-      <c r="F127" s="9"/>
-      <c r="G127" s="61"/>
-    </row>
-    <row r="128" spans="5:7">
-      <c r="E128" s="59"/>
-      <c r="F128" s="9"/>
-      <c r="G128" s="61"/>
-    </row>
-    <row r="129" spans="4:12">
-      <c r="E129" s="59"/>
-      <c r="F129" s="9"/>
-      <c r="G129" s="61"/>
-      <c r="I129" s="60"/>
-    </row>
-    <row r="130" spans="4:12">
-      <c r="E130" s="59"/>
-      <c r="F130" s="9"/>
-      <c r="G130" s="60"/>
-      <c r="H130" s="61"/>
-    </row>
-    <row r="131" spans="4:12">
-      <c r="E131" s="59"/>
-      <c r="F131" s="9"/>
-      <c r="G131" s="60"/>
-    </row>
-    <row r="132" spans="4:12">
-      <c r="E132" s="59"/>
-      <c r="F132" s="9"/>
-      <c r="G132" s="61"/>
-    </row>
-    <row r="133" spans="4:12">
-      <c r="E133" s="59"/>
-      <c r="F133" s="9"/>
-      <c r="G133" s="61"/>
-    </row>
-    <row r="134" spans="4:12">
-      <c r="E134" s="59"/>
-      <c r="F134" s="9"/>
-      <c r="G134" s="61"/>
-    </row>
-    <row r="135" spans="4:12">
-      <c r="E135" s="59"/>
-      <c r="F135" s="9"/>
-      <c r="G135" s="61"/>
-    </row>
-    <row r="136" spans="4:12">
-      <c r="E136" s="59"/>
-      <c r="F136" s="9"/>
-      <c r="G136" s="61"/>
-    </row>
-    <row r="139" spans="4:12">
-      <c r="D139" s="43"/>
-      <c r="K139" s="9" t="s">
+      <c r="G118" s="56"/>
+    </row>
+    <row r="121" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C121" s="20"/>
+      <c r="D121" s="85"/>
+      <c r="K121" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="L139">
+      <c r="L121">
         <v>6124</v>
       </c>
     </row>
-    <row r="140" spans="4:12">
-      <c r="G140" s="61"/>
-    </row>
-    <row r="141" spans="4:12">
-      <c r="G141" s="61"/>
-    </row>
-    <row r="142" spans="4:12">
-      <c r="G142" s="61"/>
-    </row>
-    <row r="143" spans="4:12">
-      <c r="G143" s="61"/>
-    </row>
-    <row r="144" spans="4:12">
-      <c r="G144" s="61"/>
-    </row>
-    <row r="145" spans="7:7">
-      <c r="G145" s="61"/>
-    </row>
-    <row r="146" spans="7:7">
-      <c r="G146" s="61"/>
-    </row>
-    <row r="147" spans="7:7">
-      <c r="G147" s="61"/>
-    </row>
-    <row r="148" spans="7:7">
-      <c r="G148" s="61"/>
-    </row>
-    <row r="149" spans="7:7">
-      <c r="G149" s="61"/>
-    </row>
-    <row r="150" spans="7:7">
-      <c r="G150" s="61"/>
-    </row>
-    <row r="151" spans="7:7">
-      <c r="G151" s="61"/>
-    </row>
-    <row r="152" spans="7:7">
-      <c r="G152" s="61"/>
-    </row>
-    <row r="153" spans="7:7">
-      <c r="G153" s="61"/>
-    </row>
-    <row r="154" spans="7:7">
-      <c r="G154" s="61"/>
-    </row>
-    <row r="155" spans="7:7">
-      <c r="G155" s="61"/>
-    </row>
-    <row r="156" spans="7:7">
-      <c r="G156" s="61"/>
-    </row>
-    <row r="157" spans="7:7">
-      <c r="G157" s="61"/>
-    </row>
-    <row r="158" spans="7:7">
-      <c r="G158" s="61"/>
-    </row>
-    <row r="159" spans="7:7">
-      <c r="G159" s="61"/>
-    </row>
-    <row r="160" spans="7:7">
-      <c r="G160" s="61"/>
-    </row>
-    <row r="161" spans="7:8">
-      <c r="G161" s="61"/>
-    </row>
-    <row r="162" spans="7:8">
-      <c r="G162" s="61"/>
-    </row>
-    <row r="163" spans="7:8">
-      <c r="G163" s="61"/>
-      <c r="H163" s="61"/>
-    </row>
-    <row r="164" spans="7:8">
-      <c r="G164" s="61"/>
-    </row>
-    <row r="165" spans="7:8">
-      <c r="G165" s="61"/>
-    </row>
-    <row r="166" spans="7:8">
-      <c r="G166" s="61"/>
-    </row>
-    <row r="167" spans="7:8">
-      <c r="G167" s="61"/>
-    </row>
-    <row r="168" spans="7:8">
-      <c r="G168" s="61"/>
-    </row>
-    <row r="169" spans="7:8">
-      <c r="G169" s="61"/>
+    <row r="122" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="G122" s="56"/>
+    </row>
+    <row r="123" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="G123" s="56"/>
+    </row>
+    <row r="124" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="G124" s="56"/>
+    </row>
+    <row r="125" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="G125" s="56"/>
+    </row>
+    <row r="126" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="G126" s="56"/>
+    </row>
+    <row r="127" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="G127" s="56"/>
+    </row>
+    <row r="128" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="G128" s="56"/>
+    </row>
+    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G129" s="56"/>
+    </row>
+    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G130" s="56"/>
+    </row>
+    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G131" s="56"/>
+    </row>
+    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G132" s="56"/>
+    </row>
+    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G133" s="56"/>
+    </row>
+    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G134" s="56"/>
+    </row>
+    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G135" s="56"/>
+    </row>
+    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G136" s="56"/>
+    </row>
+    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G137" s="56"/>
+    </row>
+    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G138" s="56"/>
+    </row>
+    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G139" s="56"/>
+    </row>
+    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G140" s="56"/>
+    </row>
+    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G141" s="56"/>
+    </row>
+    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G142" s="56"/>
+    </row>
+    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G143" s="56"/>
+    </row>
+    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G144" s="56"/>
+    </row>
+    <row r="145" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G145" s="56"/>
+      <c r="H145" s="56"/>
+    </row>
+    <row r="146" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G146" s="56"/>
+    </row>
+    <row r="147" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G147" s="56"/>
+    </row>
+    <row r="148" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G148" s="56"/>
+    </row>
+    <row r="149" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G149" s="56"/>
+    </row>
+    <row r="150" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G150" s="56"/>
+    </row>
+    <row r="151" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G151" s="56"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B105:B112"/>
     <mergeCell ref="B79:B104"/>
     <mergeCell ref="D1:L1"/>
     <mergeCell ref="B4:B28"/>
@@ -4962,711 +5033,711 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="20" customWidth="1"/>
     <col min="2" max="256" width="11.42578125" style="20" customWidth="1"/>
     <col min="257" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="21" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="21" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="21" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="21" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="21" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="21" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="21" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="21" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="21" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="21" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="21" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" s="21" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="21" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="21" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="21" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="21" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="21" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="21" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="21" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="21" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="21" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="21" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="21" t="s">
         <v>12</v>
       </c>
@@ -5679,12 +5750,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="256" width="11.42578125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Version string added on wafer maps
</commit_message>
<xml_diff>
--- a/waferstatus_20150612.xlsx
+++ b/waferstatus_20150612.xlsx
@@ -867,9 +867,6 @@
     <t>was missing in the list!</t>
   </si>
   <si>
-    <t>Waferstatus 12.06.2015 (PSI46dig V2.1respin)</t>
-  </si>
-  <si>
     <t>8 Stück</t>
   </si>
   <si>
@@ -898,6 +895,9 @@
   </si>
   <si>
     <t>VN6CDCX</t>
+  </si>
+  <si>
+    <t>Waferstatus 25.06.2015 (PSI46dig V2.1respin)</t>
   </si>
 </sst>
 </file>
@@ -1289,6 +1289,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1310,7 +1311,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1618,10 +1618,10 @@
   <dimension ref="B1:P151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N111" sqref="N111"/>
+      <selection pane="bottomRight" activeCell="B79" sqref="B79:P112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1642,17 +1642,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D1" s="81" t="s">
-        <v>282</v>
-      </c>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
+      <c r="D1" s="82" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
     </row>
     <row r="2" spans="2:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -1701,7 +1701,7 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="79" t="s">
         <v>172</v>
       </c>
       <c r="C4" s="31">
@@ -1730,7 +1730,7 @@
       <c r="P4" s="58"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="79"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="32">
         <v>2</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="P5" s="58"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="79"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="32">
         <v>3</v>
       </c>
@@ -1784,7 +1784,7 @@
       <c r="P6" s="58"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B7" s="79"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="32">
         <v>4</v>
       </c>
@@ -1811,7 +1811,7 @@
       <c r="P7" s="58"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B8" s="79"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="32">
         <v>5</v>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="P8" s="58"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="79"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="32">
         <v>6</v>
       </c>
@@ -1868,7 +1868,7 @@
       <c r="P9" s="58"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="79"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="32">
         <v>7</v>
       </c>
@@ -1898,7 +1898,7 @@
       <c r="P10" s="58"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B11" s="79"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="32">
         <v>8</v>
       </c>
@@ -1928,7 +1928,7 @@
       <c r="P11" s="58"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B12" s="79"/>
+      <c r="B12" s="80"/>
       <c r="C12" s="32">
         <v>9</v>
       </c>
@@ -1958,7 +1958,7 @@
       <c r="P12" s="58"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B13" s="79"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="32">
         <v>10</v>
       </c>
@@ -1990,7 +1990,7 @@
       <c r="P13" s="58"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="79"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="32">
         <v>11</v>
       </c>
@@ -2022,7 +2022,7 @@
       <c r="P14" s="58"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="79"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="32">
         <v>12</v>
       </c>
@@ -2054,7 +2054,7 @@
       <c r="P15" s="58"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B16" s="79"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="32">
         <v>13</v>
       </c>
@@ -2086,7 +2086,7 @@
       <c r="P16" s="58"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="79"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="32">
         <v>14</v>
       </c>
@@ -2118,7 +2118,7 @@
       <c r="P17" s="58"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="79"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="32">
         <v>15</v>
       </c>
@@ -2148,7 +2148,7 @@
       <c r="P18" s="58"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="79"/>
+      <c r="B19" s="80"/>
       <c r="C19" s="32">
         <v>16</v>
       </c>
@@ -2178,7 +2178,7 @@
       <c r="P19" s="58"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="79"/>
+      <c r="B20" s="80"/>
       <c r="C20" s="32">
         <v>17</v>
       </c>
@@ -2208,7 +2208,7 @@
       <c r="P20" s="58"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="79"/>
+      <c r="B21" s="80"/>
       <c r="C21" s="32">
         <v>18</v>
       </c>
@@ -2238,7 +2238,7 @@
       <c r="P21" s="58"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="79"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="32">
         <v>19</v>
       </c>
@@ -2268,7 +2268,7 @@
       <c r="P22" s="58"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="79"/>
+      <c r="B23" s="80"/>
       <c r="C23" s="32">
         <v>20</v>
       </c>
@@ -2298,7 +2298,7 @@
       <c r="P23" s="58"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="79"/>
+      <c r="B24" s="80"/>
       <c r="C24" s="32">
         <v>21</v>
       </c>
@@ -2328,7 +2328,7 @@
       <c r="P24" s="58"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="79"/>
+      <c r="B25" s="80"/>
       <c r="C25" s="32">
         <v>22</v>
       </c>
@@ -2358,7 +2358,7 @@
       <c r="P25" s="58"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="79"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="32">
         <v>23</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="P26" s="58"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="79"/>
+      <c r="B27" s="80"/>
       <c r="C27" s="32">
         <v>24</v>
       </c>
@@ -2419,7 +2419,7 @@
       <c r="P27" s="58"/>
     </row>
     <row r="28" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="80"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="33">
         <v>25</v>
       </c>
@@ -2463,7 +2463,7 @@
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="78" t="s">
+      <c r="B29" s="79" t="s">
         <v>179</v>
       </c>
       <c r="C29" s="44">
@@ -2495,7 +2495,7 @@
       <c r="P29" s="58"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="83"/>
+      <c r="B30" s="84"/>
       <c r="C30" s="42">
         <v>27</v>
       </c>
@@ -2525,7 +2525,7 @@
       <c r="P30" s="58"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B31" s="83"/>
+      <c r="B31" s="84"/>
       <c r="C31" s="42">
         <v>28</v>
       </c>
@@ -2555,7 +2555,7 @@
       <c r="P31" s="58"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B32" s="83"/>
+      <c r="B32" s="84"/>
       <c r="C32" s="42">
         <v>29</v>
       </c>
@@ -2585,7 +2585,7 @@
       <c r="P32" s="58"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B33" s="83"/>
+      <c r="B33" s="84"/>
       <c r="C33" s="42">
         <v>30</v>
       </c>
@@ -2615,7 +2615,7 @@
       <c r="P33" s="58"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B34" s="83"/>
+      <c r="B34" s="84"/>
       <c r="C34" s="42">
         <v>31</v>
       </c>
@@ -2645,7 +2645,7 @@
       <c r="P34" s="58"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B35" s="83"/>
+      <c r="B35" s="84"/>
       <c r="C35" s="42">
         <v>32</v>
       </c>
@@ -2675,7 +2675,7 @@
       <c r="P35" s="58"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B36" s="83"/>
+      <c r="B36" s="84"/>
       <c r="C36" s="42">
         <v>33</v>
       </c>
@@ -2705,7 +2705,7 @@
       <c r="P36" s="58"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B37" s="83"/>
+      <c r="B37" s="84"/>
       <c r="C37" s="42">
         <v>34</v>
       </c>
@@ -2735,7 +2735,7 @@
       <c r="P37" s="58"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B38" s="83"/>
+      <c r="B38" s="84"/>
       <c r="C38" s="42">
         <v>35</v>
       </c>
@@ -2765,7 +2765,7 @@
       <c r="P38" s="58"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B39" s="83"/>
+      <c r="B39" s="84"/>
       <c r="C39" s="42">
         <v>36</v>
       </c>
@@ -2795,7 +2795,7 @@
       <c r="P39" s="58"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B40" s="83"/>
+      <c r="B40" s="84"/>
       <c r="C40" s="42">
         <v>37</v>
       </c>
@@ -2827,7 +2827,7 @@
       <c r="P40" s="58"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B41" s="83"/>
+      <c r="B41" s="84"/>
       <c r="C41" s="42">
         <v>38</v>
       </c>
@@ -2857,7 +2857,7 @@
       <c r="P41" s="58"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B42" s="83"/>
+      <c r="B42" s="84"/>
       <c r="C42" s="42">
         <v>39</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="P42" s="58"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B43" s="83"/>
+      <c r="B43" s="84"/>
       <c r="C43" s="42">
         <v>40</v>
       </c>
@@ -2917,7 +2917,7 @@
       <c r="P43" s="58"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B44" s="83"/>
+      <c r="B44" s="84"/>
       <c r="C44" s="42">
         <v>41</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="P44" s="58"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B45" s="83"/>
+      <c r="B45" s="84"/>
       <c r="C45" s="42">
         <v>42</v>
       </c>
@@ -2977,7 +2977,7 @@
       <c r="P45" s="58"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B46" s="83"/>
+      <c r="B46" s="84"/>
       <c r="C46" s="42">
         <v>43</v>
       </c>
@@ -3007,7 +3007,7 @@
       <c r="P46" s="58"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B47" s="83"/>
+      <c r="B47" s="84"/>
       <c r="C47" s="42">
         <v>44</v>
       </c>
@@ -3037,7 +3037,7 @@
       <c r="P47" s="58"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B48" s="83"/>
+      <c r="B48" s="84"/>
       <c r="C48" s="42">
         <v>45</v>
       </c>
@@ -3067,7 +3067,7 @@
       <c r="P48" s="58"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B49" s="83"/>
+      <c r="B49" s="84"/>
       <c r="C49" s="42">
         <v>46</v>
       </c>
@@ -3097,7 +3097,7 @@
       <c r="P49" s="58"/>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="83"/>
+      <c r="B50" s="84"/>
       <c r="C50" s="42">
         <v>47</v>
       </c>
@@ -3127,7 +3127,7 @@
       <c r="P50" s="58"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B51" s="84"/>
+      <c r="B51" s="85"/>
       <c r="C51" s="48">
         <v>48</v>
       </c>
@@ -3169,7 +3169,7 @@
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B52" s="78" t="s">
+      <c r="B52" s="79" t="s">
         <v>208</v>
       </c>
       <c r="C52" s="44">
@@ -3202,7 +3202,7 @@
       <c r="P52" s="58"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B53" s="84"/>
+      <c r="B53" s="85"/>
       <c r="C53" s="48">
         <v>50</v>
       </c>
@@ -3245,7 +3245,7 @@
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B54" s="78" t="s">
+      <c r="B54" s="79" t="s">
         <v>172</v>
       </c>
       <c r="C54" s="44">
@@ -3274,7 +3274,7 @@
       <c r="P54" s="58"/>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B55" s="79"/>
+      <c r="B55" s="80"/>
       <c r="C55" s="42">
         <v>52</v>
       </c>
@@ -3301,7 +3301,7 @@
       <c r="P55" s="58"/>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B56" s="79"/>
+      <c r="B56" s="80"/>
       <c r="C56" s="42">
         <v>53</v>
       </c>
@@ -3328,7 +3328,7 @@
       <c r="P56" s="58"/>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B57" s="79"/>
+      <c r="B57" s="80"/>
       <c r="C57" s="42">
         <v>54</v>
       </c>
@@ -3355,7 +3355,7 @@
       <c r="P57" s="58"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B58" s="79"/>
+      <c r="B58" s="80"/>
       <c r="C58" s="42">
         <v>55</v>
       </c>
@@ -3382,7 +3382,7 @@
       <c r="P58" s="58"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B59" s="79"/>
+      <c r="B59" s="80"/>
       <c r="C59" s="42">
         <v>56</v>
       </c>
@@ -3409,7 +3409,7 @@
       <c r="P59" s="58"/>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B60" s="79"/>
+      <c r="B60" s="80"/>
       <c r="C60" s="42">
         <v>57</v>
       </c>
@@ -3436,7 +3436,7 @@
       <c r="P60" s="58"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B61" s="79"/>
+      <c r="B61" s="80"/>
       <c r="C61" s="42">
         <v>58</v>
       </c>
@@ -3463,7 +3463,7 @@
       <c r="P61" s="58"/>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B62" s="79"/>
+      <c r="B62" s="80"/>
       <c r="C62" s="42">
         <v>59</v>
       </c>
@@ -3490,7 +3490,7 @@
       <c r="P62" s="58"/>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B63" s="79"/>
+      <c r="B63" s="80"/>
       <c r="C63" s="42">
         <v>60</v>
       </c>
@@ -3517,7 +3517,7 @@
       <c r="P63" s="58"/>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B64" s="79"/>
+      <c r="B64" s="80"/>
       <c r="C64" s="42">
         <v>61</v>
       </c>
@@ -3544,7 +3544,7 @@
       <c r="P64" s="58"/>
     </row>
     <row r="65" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B65" s="79"/>
+      <c r="B65" s="80"/>
       <c r="C65" s="42">
         <v>62</v>
       </c>
@@ -3571,7 +3571,7 @@
       <c r="P65" s="58"/>
     </row>
     <row r="66" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B66" s="79"/>
+      <c r="B66" s="80"/>
       <c r="C66" s="42">
         <v>63</v>
       </c>
@@ -3598,7 +3598,7 @@
       <c r="P66" s="58"/>
     </row>
     <row r="67" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B67" s="79"/>
+      <c r="B67" s="80"/>
       <c r="C67" s="42">
         <v>64</v>
       </c>
@@ -3625,7 +3625,7 @@
       <c r="P67" s="58"/>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B68" s="79"/>
+      <c r="B68" s="80"/>
       <c r="C68" s="42">
         <v>65</v>
       </c>
@@ -3652,7 +3652,7 @@
       <c r="P68" s="58"/>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B69" s="79"/>
+      <c r="B69" s="80"/>
       <c r="C69" s="42">
         <v>66</v>
       </c>
@@ -3679,7 +3679,7 @@
       <c r="P69" s="58"/>
     </row>
     <row r="70" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B70" s="79"/>
+      <c r="B70" s="80"/>
       <c r="C70" s="42">
         <v>67</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="P70" s="58"/>
     </row>
     <row r="71" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B71" s="79"/>
+      <c r="B71" s="80"/>
       <c r="C71" s="42">
         <v>68</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="P71" s="58"/>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B72" s="79"/>
+      <c r="B72" s="80"/>
       <c r="C72" s="42">
         <v>69</v>
       </c>
@@ -3762,7 +3762,7 @@
       <c r="P72" s="58"/>
     </row>
     <row r="73" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B73" s="79"/>
+      <c r="B73" s="80"/>
       <c r="C73" s="42">
         <v>70</v>
       </c>
@@ -3791,7 +3791,7 @@
       <c r="P73" s="58"/>
     </row>
     <row r="74" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B74" s="79"/>
+      <c r="B74" s="80"/>
       <c r="C74" s="42">
         <v>71</v>
       </c>
@@ -3818,7 +3818,7 @@
       <c r="P74" s="58"/>
     </row>
     <row r="75" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B75" s="79"/>
+      <c r="B75" s="80"/>
       <c r="C75" s="42">
         <v>72</v>
       </c>
@@ -3845,7 +3845,7 @@
       <c r="P75" s="58"/>
     </row>
     <row r="76" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B76" s="79"/>
+      <c r="B76" s="80"/>
       <c r="C76" s="42">
         <v>73</v>
       </c>
@@ -3872,7 +3872,7 @@
       <c r="P76" s="58"/>
     </row>
     <row r="77" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B77" s="79"/>
+      <c r="B77" s="80"/>
       <c r="C77" s="42">
         <v>74</v>
       </c>
@@ -3899,7 +3899,7 @@
       <c r="P77" s="58"/>
     </row>
     <row r="78" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B78" s="80"/>
+      <c r="B78" s="81"/>
       <c r="C78" s="48">
         <v>75</v>
       </c>
@@ -3940,7 +3940,7 @@
       </c>
     </row>
     <row r="79" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="78" t="s">
+      <c r="B79" s="79" t="s">
         <v>172</v>
       </c>
       <c r="C79" s="44">
@@ -3969,7 +3969,7 @@
       <c r="P79" s="58"/>
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B80" s="79"/>
+      <c r="B80" s="80"/>
       <c r="C80" s="42">
         <v>77</v>
       </c>
@@ -3998,7 +3998,7 @@
       <c r="P80" s="58"/>
     </row>
     <row r="81" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B81" s="79"/>
+      <c r="B81" s="80"/>
       <c r="C81" s="42">
         <v>78</v>
       </c>
@@ -4025,7 +4025,7 @@
       <c r="P81" s="58"/>
     </row>
     <row r="82" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B82" s="79"/>
+      <c r="B82" s="80"/>
       <c r="C82" s="42">
         <v>79</v>
       </c>
@@ -4052,7 +4052,7 @@
       <c r="P82" s="58"/>
     </row>
     <row r="83" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B83" s="79"/>
+      <c r="B83" s="80"/>
       <c r="C83" s="42">
         <v>80</v>
       </c>
@@ -4079,7 +4079,7 @@
       <c r="P83" s="58"/>
     </row>
     <row r="84" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B84" s="79"/>
+      <c r="B84" s="80"/>
       <c r="C84" s="42">
         <v>81</v>
       </c>
@@ -4106,7 +4106,7 @@
       <c r="P84" s="58"/>
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B85" s="79"/>
+      <c r="B85" s="80"/>
       <c r="C85" s="42">
         <v>82</v>
       </c>
@@ -4133,7 +4133,7 @@
       <c r="P85" s="58"/>
     </row>
     <row r="86" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B86" s="79"/>
+      <c r="B86" s="80"/>
       <c r="C86" s="42">
         <v>83</v>
       </c>
@@ -4160,7 +4160,7 @@
       <c r="P86" s="58"/>
     </row>
     <row r="87" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B87" s="79"/>
+      <c r="B87" s="80"/>
       <c r="C87" s="42">
         <v>84</v>
       </c>
@@ -4189,7 +4189,7 @@
       <c r="P87" s="58"/>
     </row>
     <row r="88" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B88" s="79"/>
+      <c r="B88" s="80"/>
       <c r="C88" s="42">
         <v>85</v>
       </c>
@@ -4216,7 +4216,7 @@
       <c r="P88" s="58"/>
     </row>
     <row r="89" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B89" s="79"/>
+      <c r="B89" s="80"/>
       <c r="C89" s="42">
         <v>86</v>
       </c>
@@ -4245,7 +4245,7 @@
       <c r="P89" s="58"/>
     </row>
     <row r="90" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B90" s="79"/>
+      <c r="B90" s="80"/>
       <c r="C90" s="42">
         <v>87</v>
       </c>
@@ -4274,7 +4274,7 @@
       <c r="P90" s="58"/>
     </row>
     <row r="91" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B91" s="79"/>
+      <c r="B91" s="80"/>
       <c r="C91" s="42">
         <v>88</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="P91" s="58"/>
     </row>
     <row r="92" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B92" s="79"/>
+      <c r="B92" s="80"/>
       <c r="C92" s="42">
         <v>89</v>
       </c>
@@ -4328,7 +4328,7 @@
       <c r="P92" s="58"/>
     </row>
     <row r="93" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B93" s="79"/>
+      <c r="B93" s="80"/>
       <c r="C93" s="42">
         <v>90</v>
       </c>
@@ -4355,7 +4355,7 @@
       <c r="P93" s="58"/>
     </row>
     <row r="94" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B94" s="79"/>
+      <c r="B94" s="80"/>
       <c r="C94" s="42">
         <v>91</v>
       </c>
@@ -4382,7 +4382,7 @@
       <c r="P94" s="58"/>
     </row>
     <row r="95" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B95" s="79"/>
+      <c r="B95" s="80"/>
       <c r="C95" s="42">
         <v>92</v>
       </c>
@@ -4409,7 +4409,7 @@
       <c r="P95" s="58"/>
     </row>
     <row r="96" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B96" s="79"/>
+      <c r="B96" s="80"/>
       <c r="C96" s="42">
         <v>93</v>
       </c>
@@ -4438,7 +4438,7 @@
       <c r="P96" s="58"/>
     </row>
     <row r="97" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B97" s="79"/>
+      <c r="B97" s="80"/>
       <c r="C97" s="42">
         <v>94</v>
       </c>
@@ -4467,7 +4467,7 @@
       <c r="P97" s="58"/>
     </row>
     <row r="98" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B98" s="79"/>
+      <c r="B98" s="80"/>
       <c r="C98" s="42">
         <v>95</v>
       </c>
@@ -4496,7 +4496,7 @@
       <c r="P98" s="58"/>
     </row>
     <row r="99" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B99" s="79"/>
+      <c r="B99" s="80"/>
       <c r="C99" s="42">
         <v>96</v>
       </c>
@@ -4525,7 +4525,7 @@
       <c r="P99" s="58"/>
     </row>
     <row r="100" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B100" s="79"/>
+      <c r="B100" s="80"/>
       <c r="C100" s="42">
         <v>97</v>
       </c>
@@ -4552,7 +4552,7 @@
       <c r="P100" s="58"/>
     </row>
     <row r="101" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B101" s="79"/>
+      <c r="B101" s="80"/>
       <c r="C101" s="42">
         <v>98</v>
       </c>
@@ -4581,7 +4581,7 @@
       <c r="P101" s="58"/>
     </row>
     <row r="102" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B102" s="79"/>
+      <c r="B102" s="80"/>
       <c r="C102" s="42">
         <v>99</v>
       </c>
@@ -4606,7 +4606,7 @@
       <c r="P102" s="58"/>
     </row>
     <row r="103" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B103" s="79"/>
+      <c r="B103" s="80"/>
       <c r="C103" s="42">
         <v>100</v>
       </c>
@@ -4631,7 +4631,7 @@
       <c r="P103" s="58"/>
     </row>
     <row r="104" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B104" s="80"/>
+      <c r="B104" s="81"/>
       <c r="C104" s="48">
         <v>101</v>
       </c>
@@ -4668,17 +4668,17 @@
       </c>
     </row>
     <row r="105" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B105" s="78" t="s">
-        <v>283</v>
+      <c r="B105" s="79" t="s">
+        <v>282</v>
       </c>
       <c r="C105" s="44">
         <v>102</v>
       </c>
       <c r="D105" s="45" t="s">
+        <v>283</v>
+      </c>
+      <c r="E105" s="17" t="s">
         <v>284</v>
-      </c>
-      <c r="E105" s="17" t="s">
-        <v>285</v>
       </c>
       <c r="F105" s="3"/>
       <c r="G105" s="6"/>
@@ -4693,15 +4693,15 @@
       <c r="P105" s="58"/>
     </row>
     <row r="106" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B106" s="79"/>
+      <c r="B106" s="80"/>
       <c r="C106" s="42">
         <v>103</v>
       </c>
       <c r="D106" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E106" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="4"/>
@@ -4716,15 +4716,15 @@
       <c r="P106" s="58"/>
     </row>
     <row r="107" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B107" s="79"/>
+      <c r="B107" s="80"/>
       <c r="C107" s="42">
         <v>104</v>
       </c>
       <c r="D107" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E107" s="19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
@@ -4739,15 +4739,15 @@
       <c r="P107" s="58"/>
     </row>
     <row r="108" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B108" s="79"/>
+      <c r="B108" s="80"/>
       <c r="C108" s="42">
         <v>105</v>
       </c>
       <c r="D108" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E108" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
@@ -4762,15 +4762,15 @@
       <c r="P108" s="58"/>
     </row>
     <row r="109" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B109" s="79"/>
+      <c r="B109" s="80"/>
       <c r="C109" s="42">
         <v>106</v>
       </c>
       <c r="D109" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E109" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
@@ -4785,15 +4785,15 @@
       <c r="P109" s="58"/>
     </row>
     <row r="110" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B110" s="79"/>
+      <c r="B110" s="80"/>
       <c r="C110" s="42">
         <v>107</v>
       </c>
       <c r="D110" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E110" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
@@ -4808,15 +4808,15 @@
       <c r="P110" s="58"/>
     </row>
     <row r="111" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B111" s="79"/>
+      <c r="B111" s="80"/>
       <c r="C111" s="42">
         <v>108</v>
       </c>
       <c r="D111" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E111" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
@@ -4831,15 +4831,15 @@
       <c r="P111" s="58"/>
     </row>
     <row r="112" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="80"/>
+      <c r="B112" s="81"/>
       <c r="C112" s="48">
         <v>109</v>
       </c>
       <c r="D112" s="49" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E112" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
@@ -4913,7 +4913,7 @@
     </row>
     <row r="121" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C121" s="20"/>
-      <c r="D121" s="85"/>
+      <c r="D121" s="78"/>
       <c r="K121" s="9" t="s">
         <v>266</v>
       </c>

</xml_diff>